<commit_message>
FIX: Make sum_assured constant
</commit_message>
<xml_diff>
--- a/lifelib/libraries/savings/CashValue_ME/model_point_samples.xlsx
+++ b/lifelib/libraries/savings/CashValue_ME/model_point_samples.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,20 +466,25 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>sum_assured</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>duration_mth</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>premium_pp</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>av_pp_init</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>accum_prem_init_pp</t>
         </is>
@@ -509,15 +514,18 @@
         <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
         <v>500000</v>
       </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
       <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -545,15 +553,18 @@
         <v>100</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
         <v>500000</v>
       </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
       <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -581,15 +592,18 @@
         <v>100</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
         <v>1000</v>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
       <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -617,15 +631,18 @@
         <v>100</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
         <v>1000</v>
       </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
       <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>